<commit_message>
Focus grab & report files
</commit_message>
<xml_diff>
--- a/knowledge-center/Work-Outcomes-Template.xlsx
+++ b/knowledge-center/Work-Outcomes-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hhsgov.sharepoint.com/sites/OfficeofFamilyAssistanceOFA-FiscalResponsibilityActof2023/Shared Documents/Fiscal Responsibility Act of 2023/Work Outcomes/PRA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krono\OneDrive\Documents\GitHub\TDPrototype\knowledge-center\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{CAFE803D-D093-4227-8829-D7E73B373786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC82AADF-2422-44CD-9DF1-76F236180AA5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4C93A9-7470-4FAB-8C6B-A594F1FE548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42060" yWindow="5070" windowWidth="43920" windowHeight="23625" tabRatio="759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLE" sheetId="1" r:id="rId1"/>
@@ -30,16 +30,16 @@
     <definedName name="HTML_OS" hidden="1">0</definedName>
     <definedName name="HTML_PathFile" hidden="1">"C:\Documents and Settings\Anne Saulnier\My Documents\tanfedit\revised\tsec1r4c_mod1.htm"</definedName>
     <definedName name="HTML_Title" hidden="1">"CHILD"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">EXAMPLE!$A$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">EXAMPLE!$A$6</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="SECTION 3" guid="{E4F6F464-F401-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="5"/>
+    <customWorkbookView name="SECTION 2" guid="{E4F6F463-F401-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="5"/>
+    <customWorkbookView name="MOE_SECTION1" guid="{485F31E0-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
+    <customWorkbookView name="MOE_SECTION2" guid="{485F31E1-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
+    <customWorkbookView name="MOE_SECTION3" guid="{485F31E2-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
     <customWorkbookView name="SECTION 1" guid="{B065B980-F71B-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="5"/>
-    <customWorkbookView name="MOE_SECTION3" guid="{485F31E2-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
-    <customWorkbookView name="MOE_SECTION2" guid="{485F31E1-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
-    <customWorkbookView name="MOE_SECTION1" guid="{485F31E0-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
-    <customWorkbookView name="SECTION 2" guid="{E4F6F463-F401-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="5"/>
-    <customWorkbookView name="SECTION 3" guid="{E4F6F464-F401-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="5">
   <si>
     <r>
       <rPr>
@@ -69,6 +69,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">PAPERWORK REDUCTION ACT OF 1995 (Pub. L. 104-13) STATEMENT OF PUBLIC BURDEN: Through this information collection, ACF is gathering information to assess and evaluate whether a State TANF program meets statutorily required participation rates. Public reporting burden for this collection of information is estimated to average 100 hours per grantee per year, including the time for reviewing instructions, gathering and maintaining the data needed, and reviewing the collection of information. This is a mandatory collection of information (42 U.S.C. § 611). An agency may not conduct or sponsor, and a person is not required to respond to, a collection of information subject to the requirements of the Paperwork Reduction Act of 1995, unless it displays a currently valid OMB control number. The OMB # is xxxx-xxxx and the expiration date is XX/XX/XXXX. If you have any comments on this collection of information, please contact the Office of Family Assistance by email at TANFdata@acf.hhs.gov. </t>
     </r>
@@ -77,6 +78,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -87,12 +89,18 @@
   <si>
     <t>yyyymm</t>
   </si>
+  <si>
+    <t>Exit Date (YYYYMM)</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -133,22 +141,31 @@
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -176,16 +193,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -629,20 +650,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IA79"/>
+  <dimension ref="A1:IA80"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="175" zoomScaleNormal="115" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:235" ht="112.5" customHeight="1">
+    <row r="1" spans="1:235" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -656,7 +677,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:235" ht="48.75" customHeight="1">
+    <row r="2" spans="1:235" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -670,15 +691,15 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:235">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>9999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:235">
+    <row r="3" spans="1:235" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -686,7 +707,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:235" ht="12" customHeight="1">
+    <row r="5" spans="1:235" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -694,7 +715,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:235" ht="12" customHeight="1">
+    <row r="6" spans="1:235" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -702,7 +723,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:235" ht="12" customHeight="1">
+    <row r="7" spans="1:235" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -710,7 +731,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:235" ht="12" customHeight="1">
+    <row r="8" spans="1:235" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -718,7 +739,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:235" ht="12" customHeight="1">
+    <row r="9" spans="1:235" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -726,7 +747,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:235">
+    <row r="10" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -734,7 +755,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:235">
+    <row r="11" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -742,7 +763,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:235" ht="12" customHeight="1">
+    <row r="12" spans="1:235" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -750,7 +771,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:235">
+    <row r="13" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -758,7 +779,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:235">
+    <row r="14" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -766,7 +787,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:235">
+    <row r="15" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -774,7 +795,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:235" s="2" customFormat="1">
+    <row r="16" spans="1:235" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -1015,7 +1036,7 @@
       <c r="HZ16" s="1"/>
       <c r="IA16" s="1"/>
     </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1">
+    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1023,7 +1044,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="13.5" customHeight="1">
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -1031,7 +1052,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -1039,7 +1060,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -1047,7 +1068,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -1055,7 +1076,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -1063,7 +1084,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
@@ -1071,7 +1092,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
@@ -1079,7 +1100,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>2</v>
       </c>
@@ -1087,7 +1108,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -1095,7 +1116,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1124,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -1111,7 +1132,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
@@ -1119,7 +1140,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
@@ -1127,7 +1148,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
@@ -1135,7 +1156,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
@@ -1143,7 +1164,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +1172,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
@@ -1159,7 +1180,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>2</v>
       </c>
@@ -1167,7 +1188,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
@@ -1175,7 +1196,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>2</v>
       </c>
@@ -1183,7 +1204,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>2</v>
       </c>
@@ -1191,7 +1212,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
@@ -1199,7 +1220,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
@@ -1207,7 +1228,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>2</v>
       </c>
@@ -1215,7 +1236,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
@@ -1223,7 +1244,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -1231,7 +1252,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
@@ -1239,7 +1260,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>2</v>
       </c>
@@ -1247,7 +1268,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>2</v>
       </c>
@@ -1255,7 +1276,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>2</v>
       </c>
@@ -1263,7 +1284,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>2</v>
       </c>
@@ -1271,7 +1292,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:235">
+    <row r="49" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>2</v>
       </c>
@@ -1279,7 +1300,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:235" ht="12" customHeight="1">
+    <row r="50" spans="1:235" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1308,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:235">
+    <row r="51" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
@@ -1295,7 +1316,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:235">
+    <row r="52" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
@@ -1303,7 +1324,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:235">
+    <row r="53" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
@@ -1311,7 +1332,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:235" s="2" customFormat="1">
+    <row r="54" spans="1:235" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>2</v>
       </c>
@@ -1552,7 +1573,7 @@
       <c r="HZ54" s="1"/>
       <c r="IA54" s="1"/>
     </row>
-    <row r="55" spans="1:235" ht="13.5" customHeight="1">
+    <row r="55" spans="1:235" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>2</v>
       </c>
@@ -1560,7 +1581,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:235" ht="13.5" customHeight="1">
+    <row r="56" spans="1:235" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>2</v>
       </c>
@@ -1568,7 +1589,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:235">
+    <row r="57" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>2</v>
       </c>
@@ -1576,7 +1597,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:235">
+    <row r="58" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>2</v>
       </c>
@@ -1584,7 +1605,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:235">
+    <row r="59" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>2</v>
       </c>
@@ -1592,7 +1613,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:235">
+    <row r="60" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>2</v>
       </c>
@@ -1600,7 +1621,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:235">
+    <row r="61" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>2</v>
       </c>
@@ -1608,7 +1629,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:235">
+    <row r="62" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>2</v>
       </c>
@@ -1616,7 +1637,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:235">
+    <row r="63" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>2</v>
       </c>
@@ -1624,7 +1645,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:235">
+    <row r="64" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>2</v>
       </c>
@@ -1632,7 +1653,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>2</v>
       </c>
@@ -1640,7 +1661,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>2</v>
       </c>
@@ -1648,7 +1669,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
@@ -1656,7 +1677,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>2</v>
       </c>
@@ -1664,7 +1685,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>2</v>
       </c>
@@ -1672,7 +1693,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>2</v>
       </c>
@@ -1680,7 +1701,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>2</v>
       </c>
@@ -1688,7 +1709,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>2</v>
       </c>
@@ -1696,7 +1717,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>2</v>
       </c>
@@ -1704,7 +1725,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>2</v>
       </c>
@@ -1712,7 +1733,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>2</v>
       </c>
@@ -1720,7 +1741,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>2</v>
       </c>
@@ -1728,7 +1749,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>2</v>
       </c>
@@ -1736,7 +1757,7 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>2</v>
       </c>
@@ -1744,17 +1765,25 @@
         <v>9999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B79" s="3">
+        <v>9999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="3">
         <v>9999999999</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B065B980-F71B-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{E4F6F464-F401-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1764,7 +1793,7 @@
         <oddFooter>&amp;L&amp;F&amp;CPage &amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{485F31E2-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{E4F6F463-F401-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1774,7 +1803,7 @@
         <oddFooter>&amp;L&amp;F&amp;CPage &amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{485F31E1-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{485F31E0-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1784,7 +1813,7 @@
         <oddFooter>&amp;L&amp;F&amp;CPage &amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{485F31E0-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{485F31E1-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1794,7 +1823,7 @@
         <oddFooter>&amp;L&amp;F&amp;CPage &amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{E4F6F463-F401-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{485F31E2-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1804,7 +1833,7 @@
         <oddFooter>&amp;L&amp;F&amp;CPage &amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{E4F6F464-F401-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{B065B980-F71B-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1821,23 +1850,23 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.2" header="0.05" footer="0.3"/>
-  <pageSetup scale="81" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
+  <pageSetup scale="54" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2018,13 +2047,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C49F0C-194B-446F-A859-45BEA59A7F08}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{947173F8-8A53-4697-8B0E-D24B110213D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{947173F8-8A53-4697-8B0E-D24B110213D9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C49F0C-194B-446F-A859-45BEA59A7F08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8E93465-BA08-4D90-952D-1AC024538CDB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8E93465-BA08-4D90-952D-1AC024538CDB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dbb6e81e-6d27-4b06-96f4-00eb39bd1984"/>
+    <ds:schemaRef ds:uri="1d2040a8-051f-4312-97c4-228835cbdc01"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>